<commit_message>
modified sprint 4 backlog
</commit_message>
<xml_diff>
--- a/Sprint_4_Backlog.xlsx
+++ b/Sprint_4_Backlog.xlsx
@@ -40,55 +40,55 @@
     <t>Lujine</t>
   </si>
   <si>
+    <t>Yasser</t>
+  </si>
+  <si>
+    <t>As an investor I should be able to view rejected forms with the lawyer's comments, so that I can know which data to update.</t>
+  </si>
+  <si>
+    <t>Mostafa</t>
+  </si>
+  <si>
+    <t>As a lawyer I should be able to send back rejected forms attached with comments to the investor, so that they can be updated appropriately.</t>
+  </si>
+  <si>
     <t>Omar</t>
   </si>
   <si>
-    <t>As an investor I should be able to view rejected forms with the lawyer's comments, so that I can know which data to update.</t>
+    <t>Farid</t>
   </si>
   <si>
     <t>Mohamed Ayman</t>
   </si>
   <si>
+    <t>As an admin I should be able to search through all cases so that I can see their details.</t>
+  </si>
+  <si>
+    <t>Adel</t>
+  </si>
+  <si>
+    <t>As a registered/unregistered user I should be able to see approved companies' E-journals so I can know information about them</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>As an internal user I should be able to log in to the internal portal so that I can work on my tasks</t>
+  </si>
+  <si>
     <t>Ahmed El-Sherif</t>
   </si>
   <si>
-    <t>As a lawyer I should be able to send back rejected forms attached with comments to the investor, so that they can be updated appropriately.</t>
-  </si>
-  <si>
-    <t>Mostafa</t>
-  </si>
-  <si>
-    <t>As an admin I should be able to search through all cases so that I can see their details.</t>
-  </si>
-  <si>
-    <t>Adel</t>
-  </si>
-  <si>
-    <t>Farid</t>
-  </si>
-  <si>
-    <t>As a registered/unregistered user I should be able to see approved companies' E-journals so I can know information about them</t>
-  </si>
-  <si>
-    <t>As an internal user I should be able to log in to the internal portal so that I can work on my tasks</t>
-  </si>
-  <si>
     <t>As an investor I should be able to register to the website so that I can join the portal and be able to establish my own companies</t>
   </si>
   <si>
     <t>As an admin I should be able to delete/deactivate the account of the employees who leave GAFI, so that I can prevent unauthorized access.</t>
   </si>
   <si>
-    <t>Yasser</t>
-  </si>
-  <si>
     <t>As an investor I should be able to see an FAQ page so that it can help me understand how the website works</t>
   </si>
   <si>
     <t>As an investor I should be able to keep track of my application, so that I can see which state my application is at.</t>
-  </si>
-  <si>
-    <t>Mark</t>
   </si>
 </sst>
 </file>
@@ -158,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -189,14 +189,17 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -276,10 +279,10 @@
       <c r="D2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="4"/>
@@ -314,11 +317,11 @@
       <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>12</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
@@ -344,19 +347,19 @@
         <v>4.11</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="7">
         <v>3.0</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -382,19 +385,19 @@
         <v>4.09</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7">
         <v>5.0</v>
       </c>
       <c r="D5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>14</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -426,13 +429,13 @@
         <v>3.0</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -458,19 +461,19 @@
         <v>5.02</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" s="7">
         <v>2.0</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>21</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -497,16 +500,16 @@
         <v>5.03</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C8" s="7">
         <v>3.0</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>8</v>
@@ -532,23 +535,23 @@
       <c r="Y8" s="8"/>
     </row>
     <row r="9">
-      <c r="A9" s="10">
+      <c r="A9" s="12">
         <v>5.05</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="13">
+        <v>3.0</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="11">
-        <v>3.0</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>11</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -571,23 +574,23 @@
       <c r="Y9" s="8"/>
     </row>
     <row r="10">
-      <c r="A10" s="13">
+      <c r="A10" s="14">
         <v>3.04</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="11">
+        <v>24</v>
+      </c>
+      <c r="C10" s="13">
         <v>3.0</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="8" t="s">
+      <c r="D10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>16</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -614,43 +617,43 @@
       <c r="AC10" s="4"/>
     </row>
     <row r="11">
-      <c r="A11" s="14">
+      <c r="A11" s="15">
         <v>3.01</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="11">
+        <v>25</v>
+      </c>
+      <c r="C11" s="13">
         <v>3.0</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
+        <v>13</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>